<commit_message>
updated instruction and method, minor changes to the UI for flow analysis
</commit_message>
<xml_diff>
--- a/inst/extdata/demo_flowrate_data.xlsx
+++ b/inst/extdata/demo_flowrate_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/rainfall_flow_calculator_shiny/demo_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/bmp-hydrology-calculator/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{E1E1FAC7-CE81-40D3-BA68-902FCADE7445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B2FC3F9-6F4F-4F0A-883A-A1CF01E12339}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{E1E1FAC7-CE81-40D3-BA68-902FCADE7445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BBDE438-AF54-4766-B8D9-15A02B45847F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,7 +178,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -187,15 +187,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Application Usage Guide</a:t>
+            <a:t>Hydrograph data can be submitted for a single rain event at one time. Up to four flows in the same event can be accommodated for analysis. The available flow types are inflow 1, inflow 2, outflow, and bypass. A user does not need to submit all four types; refer to the Methods tab for an illustration of common BMP flow type configurations. If any of the data types are not applicable, leave the tab blank (as is).</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -204,15 +201,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>=======================</a:t>
+            <a:t>Download flow demo data</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -221,15 +215,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>This guide provides instructions for using the application and outlines the data requirements for successful analysis.</a:t>
+            <a:t>Download flow template</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1600" b="1" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -238,15 +229,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Analysis Types</a:t>
+            <a:t>Data Requirements:</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -255,15 +241,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>--------------</a:t>
+            <a:t> There are 5 worksheets in the data template: instructions, inflow1, inflow2, outflow, bypass. The uploaded Excel spreadsheet must conform to the following requirements:</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -272,15 +255,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>IMPORTANT: The column names and tab names in the templates (both rainfall and flow) must remain unchanged for accurate analysis and app's functionality.</a:t>
+            <a:t>Each tab must contain exactly two columns, one for the measured timestamps data and one for the associated values.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -289,15 +269,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The application supports two types of analysis: Rainfall Analysis and Flow Analysis. </a:t>
+            <a:t>The timestamp should be in 24-hour format (mm/dd/yy hh:mm:ss).</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -306,15 +283,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>---------------------</a:t>
+            <a:t>All tabs must use the same flow unit. Flow data must be in units of L/s, gpm, or cfs.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
+            <a:rPr lang="en-US" sz="1600" b="1" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -323,321 +297,16 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Rainfall Analysis</a:t>
+            <a:t>Do not change the column names and the tab names from the template.</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: The user is advised to copy and paste the rainfall data, whether it is in the form of 1-minute or time-of-tips data, into the downloaded template. It is important to note that the rain gauge values must be entered into the designated rain column within the template. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>A user can submit a continuous rainfall record without skipping any timestamps, containing multiple events in a single file.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
+          <a:endParaRPr lang="en-US" sz="1600" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
             <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Demo data are available on the Shin</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>y App.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>---------------------</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Flow</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Analysis</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: Flow data should be copy-pasted from the user's datasheet to the downloaded data template. Up to four flows can be accomodated for analysis. The available flow types are inflow 1, inflow 2, outflow and bypass. Refer to the Methods tab for an illustration of the possible flow type configurations. A user does not need to submit all four types, any combination of the flow types is acceptable. A user can only submit flow data for a single rain event. If any of the data types are not applicable, leave the tab blank (as is)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Demo data are available on the Shin</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>y App.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>---------------------</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Data Requirements</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>---------------------</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>To ensure successful analysis, the uploaded Excel spreadsheet must conform to the following requirements:</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Flow must be reported in units of L/s, gpm, or cfs.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- The timestamp should be in 24-hour format (mm/dd/yy hh:mm:ss).</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Each tab must contain exactly two columns: one for the sample timestamps data and one for the associated values.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- The column names and the tab names must not be changed from the template.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Please ensure that your data meets these requirements before using the application for analysis.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>For further assistance or inquiries, please contact our support team at stormwater@sccwrp.org</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -936,7 +605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE88C01-577A-4903-8B8F-8FB963800B71}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -64110,22 +63781,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <OldForms xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75e20f4bf570a29fdd68b6ac0ce9f23e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d8333fcdd8157586878df4d15f204f2" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cdbf04b8ff6af1f1edbadfc0fb707b99">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f194f4ff1faacf22d916baffc85e0afb" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
     <xsd:import namespace="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
@@ -64154,6 +63820,7 @@
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:OldForms" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -64254,6 +63921,11 @@
         <xsd:restriction base="dms:Text">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="28" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -64398,15 +64070,32 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <OldForms xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6636DA7F-7D61-4910-9C4D-7AB6320A82E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0282FC7-64ED-46FA-83B8-A0CD2CBEE49F}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFAD6E13-0CB9-4AE0-A0AB-1C1C6356142E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -64416,16 +64105,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA300DFB-8FA6-4B8C-AABC-4A35878068E3}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6636DA7F-7D61-4910-9C4D-7AB6320A82E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>